<commit_message>
Data for Experiment 5 and 6.
</commit_message>
<xml_diff>
--- a/Experiment_05/Lab5 NPN and PNP.xlsx
+++ b/Experiment_05/Lab5 NPN and PNP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmust-my.sharepoint.com/personal/1220031811_student_must_edu_mo/Documents/3rd Yr. in MUST/EIE341 Analog Circuit Experiment/Experiment_05/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive-Macau University of Science and Technology\OneDrive - Macau University of Science and Technology\3rd Yr. in MUST\EIE341 Analog Circuit Experiment\Experiment_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_F25DC773A252ABDACC104849719A52565BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02D7419E-4457-4572-BD94-AFB7C384AD0F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47072D51-C4E9-49D4-B969-2439F8CCD8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5835" yWindow="1605" windowWidth="22065" windowHeight="12750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>NPN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,6 +36,10 @@
   </si>
   <si>
     <t>Vo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PNP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -361,20 +365,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -388,114 +392,143 @@
         <v>0.5</v>
       </c>
       <c r="E2">
+        <v>0.6</v>
+      </c>
+      <c r="F2">
         <v>0.75</v>
       </c>
-      <c r="F2">
+      <c r="G2">
+        <v>0.82</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>1.2</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>1.3</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>1.4</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>1.5</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>1.55</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>1.6</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>1.65</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>1.7</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>1.75</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>1.8</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>1.9</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>2</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>3</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>4</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>4.91</v>
+      </c>
+      <c r="C3">
+        <v>4.91</v>
+      </c>
+      <c r="D3">
+        <v>4.91</v>
+      </c>
+      <c r="E3">
+        <v>4.78</v>
+      </c>
       <c r="F3">
+        <v>4.22</v>
+      </c>
+      <c r="G3">
+        <v>3.85</v>
+      </c>
+      <c r="H3">
         <v>2.25</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>2.0299999999999998</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>1.47</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0.95</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>0.54</v>
-      </c>
-      <c r="K3">
-        <v>0.24</v>
-      </c>
-      <c r="L3">
-        <v>0.32</v>
       </c>
       <c r="M3">
         <v>0.24</v>
       </c>
       <c r="N3">
+        <v>0.32</v>
+      </c>
+      <c r="O3">
+        <v>0.24</v>
+      </c>
+      <c r="P3">
         <v>0.21</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>0.2</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>0.191</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>0.18099999999999999</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>1.171</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>0.16300000000000001</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>0.123</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <v>0.106</v>
       </c>
-      <c r="V3">
+      <c r="X3">
         <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>